<commit_message>
sending emails to multiple recipients
</commit_message>
<xml_diff>
--- a/Mail/contents.xlsx
+++ b/Mail/contents.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="6540" yWindow="500" windowWidth="19180" windowHeight="15940"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Mail Address</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -61,15 +61,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>icists@icists.org</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>박기현, EX 권기훈, icists, 2019년 2월 14일(목), 권기훈</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>#</t>
+    <t>icists@icists.org, media@icists.org</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -442,7 +438,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -472,26 +468,23 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" display="icists@icists.org"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>